<commit_message>
added CLI interface to run scripts + started working on preprocessing tool
</commit_message>
<xml_diff>
--- a/data/test_interviews.xlsx
+++ b/data/test_interviews.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://undp.sharepoint.com/sites/BusinessEarlyRecovery/Shared Documents/General/Afghanistan/Agriculture/Cotton &amp; Dairy Value Chain Analysis/04_data_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulvercoustre/Documents/data_science/LLMs/qual_coder/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{35BD9EF1-FA29-8E48-8E53-3500C408B97A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AB497E7-9D72-CF42-872A-3684CFA6ABED}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EBFD45-817D-9343-A926-6D0E32BE2ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33640" yWindow="5240" windowWidth="29660" windowHeight="20920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Question</t>
   </si>
@@ -61,48 +61,6 @@
     <t>1.2 What are the linkages between core value chain actors?</t>
   </si>
   <si>
-    <t>1.3 In your section in the value chain, what are the supporting actors/services that are currently available?</t>
-  </si>
-  <si>
-    <t>1.4 What roles do women have in the value chain?</t>
-  </si>
-  <si>
-    <t>2.1 Describe the various activities that your firms currently perform as part of their operations?</t>
-  </si>
-  <si>
-    <t>2.2 What is the labor force involved in your operations?</t>
-  </si>
-  <si>
-    <t>2.3 What machinery (if any) do you use as part of your operations?</t>
-  </si>
-  <si>
-    <t>2.4 What challenges (if any) do you face in selling your products/services?</t>
-  </si>
-  <si>
-    <t>2.5 What challenges (if any) do you face in accessing the necessary inputs for your operations?</t>
-  </si>
-  <si>
-    <t>2.6 What challenges (if any) do you face in conducting your operational processes?</t>
-  </si>
-  <si>
-    <t>2.7 What solutions or opportunities do you see to address these challenges and improve value addition in your operations?</t>
-  </si>
-  <si>
-    <t>2.8 What would be needed to implement these opportunities and improvements in value addition?</t>
-  </si>
-  <si>
-    <t>3.1 What support services are currently missing to conduct your operations? What challenges (if any) do you face in accessing support services?</t>
-  </si>
-  <si>
-    <t>3.2 How is the (business) environment impacting your operations?</t>
-  </si>
-  <si>
-    <t>3.2 What changes to support services and the business environment would help your business the most?</t>
-  </si>
-  <si>
-    <t>Any other remarks?</t>
-  </si>
-  <si>
     <t>Tahir Faizi</t>
   </si>
   <si>
@@ -131,48 +89,6 @@
   </si>
   <si>
     <t>Linkages: 1. Dairy Farmers ↔ Input Suppliers: Transactions: Farmers purchase straw and concentrate from input suppliers. Average Prices: Wheat Straw: 24,000 AF per cow per year (3,360 kg/ 7AFN). Concentrate: 27,500 AF per cow per year (1,400 kg/ 19AFN). Dry Bread: 14,600 AF per cow per year (730 kg/ 20AFN). 2. Dairy Farmers ↔ Veterinarians: Transactions: Farmers seek health services, including vaccinations and artificial insemination. Types: Payment for services, information exchange about animal health. 3. Dairy Farmers ↔ Milk Collection Center: Transactions: Sales of milk to the collection center. Type: Buying and selling relationship, with potential for quality feedback. 4. Milk Collection Center ↔ Balkh Dairy Company: Transactions: Transfer of milk from the collection center to the dairy company for processing. Type: Supply chain relationship. 5. Dairy Farmers ↔ Equipment Suppliers: Transactions: Purchase of milking machines and processing equipment. Type: Buying relationship for necessary operational tools. Integration: Horizontal Integration: Limited coordination among farmers; some may collaborate in informal groups but not in formal cooperatives. Vertical Integration: There is a clear coordination between farmers and input suppliers, veterinarians, and the milk collection center, facilitating a structured supply chain.</t>
-  </si>
-  <si>
-    <t>Available Supporting Actors/Services: 1. Government Support: Services: Last year, the government distributed a 50 kg pack of concentrate to  of households in the district. However, this was minimal and often insufficient. Limitations: Farmers mainly bear costs for disease treatment, vaccination, artificial insemination, and nutrition. 2. Transportation Services: Means Used: Transportation is primarily conducted using rickshaws and taxis, which are inadequate for large-scale operations. 3. Storage Services: Limitations: There are no facilities for milk storage at home due to lack of electricity, refrigerators, and preservatives. 4. Market Access: Current Market: Farmers primarily rely on the milk collection center for sales. Market Information: There is a lack of knowledge regarding broader market access and information. 5. Training Needs: Marketing Support: Farmers express a need for training in marketing processes, including how to pack and preserve milk to enhance sales.</t>
-  </si>
-  <si>
-    <t>Involvement of Women: Functions: Milking: Women primarily handle the milking of cows. Dairy Processing: They are also engaged in processing dairy products, such as yogurt. Animal Care: A small percentage of women participate in feeding and cleaning the animals. Exclusion from Certain Roles: Fodder Production: Women do not participate in the production and preparation of animal feed. Marketing and Sales: All marketing and sales activities are conducted by men, limiting women's involvement in these critical areas. Reasons for Limited Participation: Cultural norms and gender roles in the community restrict women from engaging in activities perceived as requiring authority or public interaction, such as marketing and sales.</t>
-  </si>
-  <si>
-    <t>Current Activities in Operations: Inputs: Consumables: Animal food (straw, concentrate, dried bread). Treatment and vaccination supplies. Artificial insemination services. Energy sources (solar, gas, fuel wood). Basic equipment (buckets, bowls). Outputs: Products: Milk. Yogurt. Process Steps: 1. Accessing Inputs: Purchase animal food and necessary supplies for treatment and energy. 2. Production: Milking cows using traditional methods. Processing milk into yogurt without proper facilities. 3. Selling Outputs: Selling milk to the collection center. Selling yogurt to local shops. Value Addition Activities: Currently, there are no implemented practices for adding value to products. The methods of milking and processing are simple and do not enhance product quality. Products spoil quickly (e.g., milk thickens and sours within a day).</t>
-  </si>
-  <si>
-    <t>Labor Force Involvement: Labor Force Composition: Each farm typically employs an average of 2 to 3 workers, primarily consisting of mothers from milk-producing households. Specific Actions/Processes: Feeding and Preparation: Workers prepare food for the animals and ensure they are fed properly. Cleaning: Regular cleaning and washing of the farm facilities to maintain hygiene. Milking and Processing: One household member focuses on milking cows, processing the milk, and packaging dairy products. Dairy Processing Tasks: Women are actively involved in: Milking cows. Heating milk. Separating cream. Preparing yogurt. Packaging yogurt for sale. Skills of the Labor Force: The labor force does not possess specialized skills; activities are conducted using simple and traditional methods. Tools and practices include: Basic feeding techniques with straw and concentrate. Use of large bowls for milking and processing. Traditional fuel sources, such as wood. Role of Women: Women play a crucial role in the labor force, primarily in milking and dairy processing activities. They are integral to the daily operations of the farm, contributing significantly to the production of milk and yogurt.</t>
-  </si>
-  <si>
-    <t>Current Machinery: The operations rely on simple, manual tools rather than specialized machinery. The primary equipment includes: 1. Milking Bucket: Action: Used for hand milking cows. Cost: Part of overall equipment, totaling around 800 AF. 2. Milk Transfer Bucket: Action: Used to transport milk to the collection center. 3. Large Processing Bowls: Action: Employed for processing milk and preparing yogurt. 4. Fuel Sources: Gas and Wood: Used for fire in processing. Cost: The total cost for all equipment does not exceed 800 AF at current rates. Capacity and Usage: Capacity: The tools do not have a specified maximum capacity, as they are used for basic operations. Utilization: The equipment is not used at maximum capacity due to the limitations of traditional practices and small-scale operations.</t>
-  </si>
-  <si>
-    <t>Market Demand Changes: 2023 vs. 2024: Demand for dairy products has decreased significantly. Sales have dropped by 50%, with previous sales of 20 kilos of milk and 10 kilos of yogurt now reduced. Challenges in Identifying/Accessing Buyers: Lack of Market: We don't know why there is no established dairy sales market in our city, making it difficult to find buyers. Marketing Issues: There is a significant lack of marketing efforts for milk and yogurt, which affects visibility and sales. We are tired because of this lack of marketing, and we don't sell as we expected. Challenges in Meeting Buyer Requirements: Quality Expectations: We often cannot meet buyer expectations for high-quality milk and yogurt due to inadequate infrastructure (e.g., no electricity, refrigeration, or proper storage). Transportation Issues: Lack of equipped transportation means products are not kept at optimal conditions, leading to spoilage. The amount of milk and its price are determined by the company, and we have to go to the milk collection center early each morning, but they often don't accept our milk. Competition: Main Competitors: Strong competition from established brands, particularly Iranian dairy products, which have better packaging, longer shelf life, and a reputation for quality. Impact of Competition: Competitors dominate the market, making it difficult for local producers to sell their products at competitive prices.</t>
-  </si>
-  <si>
-    <t>Challenges in Accessing Necessary Inputs: Availability of Inputs: Daily inputs primarily consist of straw and concentrate, which are generally available in the field. Affordability of Inputs: While the quality of inputs is satisfactory, the cost is higher than the output generated from milk and yogurt sales. This imbalance creates financial strain on operations. Quality of Inputs: The quality of straw and concentrate meets the basic nutritional needs of the animals, but the costs associated with these inputs limit profitability. Specific Requirements: The current inputs do not maximize output potential. Although available materials meet the animals' nutritional needs, they do not lead to the expected production levels.</t>
-  </si>
-  <si>
-    <t>Challenges in Conducting Operational Processes: Access to Equipment/Technology/Machinery: The equipment currently in use is simple and local, consisting mainly of buckets, pans, and pots. This equipment does not meet essential operational needs, particularly in terms of storage and packaging. Impact: The lack of adequate storage and packaging leads to spoilage and fermentation of products, which severely compromises the quality of milk and yogurt. This results in reduced sales and profitability. Access to Labor Skills: While basic veterinary services are available for disease treatment, vaccination, and artificial insemination, there is dissatisfaction with the quality of these services. The performance of veterinarians is often lacking, which affects animal health and productivity. Impact: Poor veterinary care can lead to increased health issues among livestock, further diminishing milk production and quality. Infrastructure Challenges: There is a significant need for improved infrastructure, including electricity and refrigeration, to maintain product quality. Additionally, proper storage facilities are lacking. Impact: Without adequate infrastructure, the ability to package products with validity dates and necessary certifications is hindered. This limitation affects marketability and compliance with buyer requirements.</t>
-  </si>
-  <si>
-    <t>Addressing Value Addition Needs: 1. Improved Storage: Better storage at milk collection centers would help preserve product quality. 2. Standard Transportation: Reliable refrigerated transport is crucial for maintaining freshness in new markets. 3. Enhanced Packaging: Upgrading packaging methods and ensuring proper labeling would increase product value. Solutions and Opportunities for Improvement: Improving Production and Operational Processes: There are opportunities to enhance production using existing land and irrigation. However, knowledge gaps exist in preparing silage fodder and using high-quality materials as alternatives to concentrate. Practical training in these areas is essential. Exploring Higher-Value Products: Low-quality raw materials like straw can potentially be transformed into higher-quality feed through urea treatment. Learning this method could boost livestock health and milk quality. New Market Opportunities: Emerging markets in Mazar-e-Sharif and Samangan present opportunities for larger sales. However, challenges remain due to inadequate standard and refrigerated transportation.</t>
-  </si>
-  <si>
-    <t>Implementation Needs for Opportunities and Improvements: Financial Support: Infrastructure Investment: Financial support is needed to improve infrastructure to compete with foreign products. This includes funding for storage facilities and transportation. Purpose: Support would facilitate the storage and distribution of milk and other products, extending their shelf life. Certifications: Standards Compliance: Meeting specific certification standards is essential for our product validity. This includes labeling with production and expiration dates to ensure safety and marketability. Technical Training: Training Areas Needed: Production and processing of high-quality, cost-effective animal feed. Animal health management, including prevention and treatment methods. Processing, and marketing strategies, including proper product handling and labeling. Role of Government, NGOs, and Private Sector: Government: The agriculture department should enhance its development and extension services to support local producers. NGOs: NGOs should assist in building infrastructure, such as strengthening milk collection centers and establishing storage facilities. They should also provide training in processing and packaging. Private Sector: Collaboration with the private sector could help produce packaging materials and develop national processing centers to improve efficiency and product quality.</t>
-  </si>
-  <si>
-    <t>Missing Support Services and Challenges: Missing Support Services: 1. Animal Feed Development: There are no services available to help producers develop high-quality animal feed. Despite having raw materials, producers struggle to effectively combine and process them. 2. Refrigerated Transportation: Standard refrigerated transportation is lacking, leading to spoilage and fermentation of products, particularly during hot weather. 3. Access to Modern Techniques: Producers lack knowledge and access to modern practices for healthy animal feeding and the preparation of combined feeds. 4. Infrastructure: Although there is running water and a favorable climate for growing fodder, suitable varieties that thrive in the local climate are not available. Challenges in Accessing Support Services: High Costs: Financial constraints limit investments in necessary infrastructure and services, impacting overall productivity. Lack of Tailored Services: Existing support services do not adequately meet the specific needs of local producers, particularly in animal health and fodder preparation. Barriers to Access: Producers face difficulties in obtaining information and resources necessary (especially financial) for extending product shelf life and maintaining quality. Impact on Business: The absence of crucial support services hampers productivity and product quality, leaving producers vulnerable to competition from imported products. Ineffective animal feeding practices and a lack of modern techniques lead to lower livestock health and productivity. Without proper transportation and storage solutions, product quality deteriorates, resulting in financial losses and diminished market competitiveness.</t>
-  </si>
-  <si>
-    <t>Impact of the Business Environment on Operations: Policies, Taxes, and Tariffs: Lack of Awareness: Producers are generally unaware of any specific taxes or tariffs that may affect their operations, making it difficult to assess their impact. Climate Change: Fodder Crop Decrease: Climate change and drought conditions have led to a significant reduction in fodder crops. This annual decline results in lower food availability for livestock. Rising Input Costs: The decrease in available fodder has increased the price of food inputs, further straining producers' resources and profitability. Infrastructure Challenges: Traditional Sheds: The use of traditional animal housing during winter leads to issues such as exposure to cold, waste accumulation, and decreased efficiency in operations. The lack of modern infrastructure exacerbates these challenges, impacting overall productivity.</t>
-  </si>
-  <si>
-    <t>Changes Needed in Support Services and Business Environment: 1. Modernize Livestock Farming: Shift from traditional methods to advanced practices for better productivity. 2. Upgrade Milking Equipment: Move from manual to machine milking to improve efficiency and reduce labor costs. 3. Improve Milk Storage: Implement modern storage solutions to maintain quality and extend shelf life. 4. Adopt Modern Sales Strategies: Transition to modern marketing and sales methods to enhance market reach. 5. Promote Local Production: Strengthen the market for local dairy products to reduce reliance on imports and boost the local economy.</t>
-  </si>
-  <si>
-    <t>Additional Topics and Challenges: 1. Lack of Support Services by NGOs: Producers are deprived of essential support services needed to enhance operations and productivity. 2. Need for a Union: There is no existing union for producers, which limits collective bargaining and support. 3. Formation of a Livestock Cooperative: Establishing a cooperative would allow producers to: Join forces to meet each other's needs. Purchase inputs collectively, reducing costs. Access new markets and sell outputs at reasonable prices. 4. Access to Small Loans: Small loans are crucial for improving living standards and optimizing labor use. With several tons of labor available in each household, access to financing would enable producers to: Increase their production levels. Expand the number of dairy cows, enhancing overall output. Overall Impact: Addressing these challenges through cooperation and financial support will significantly improve our productivity, market access, and the economic well-being of all dairy producers.</t>
   </si>
   <si>
     <t>FGD-FAF-1</t>
@@ -222,215 +138,6 @@
 o	Coordination: Direct coordination exists between milk sellers and farmers for buying and selling milk, facilitating smooth transactions.
 6.	Vertical Integration:
 o	Coordination: Indirect coordination occurs between farmers, large dairy companies, and consumers, creating a structured supply chain.</t>
-  </si>
-  <si>
-    <t>Supporting Actors/Services in the Value Chain
-1.	Financial Services:
-o	Availability: No formal financial support is available in the region.
-o	Details: There are no government initiatives or small loan banks offering support for livestock owners. However, some dairy actors provide prepayment loans during the spring season when needed.
-2.	Transportation and Storage Services:
-o	Availability: there are lake of sufficient transportation and storge facilities.
-3.	Extension Services:
-o	Availability: Limited access.
-o	Details: There are not enough agricultural extension services available to provide support or guidance to farmers.
-4.	Market Access and Information:
-o	Availability: Limited access.
-o	Details: There are no formal marketing services for dairy products, which affects market access and information dissemination.
-5.	Certification Services:
-o	Details: There are no certification services  for dairy products in the region because we don’t know about how to do it.
-6.	Support from Ministries or NGOs:
-o	Availability: Availability: Limited access.
-o	Details: No collaboration or support from government ministries, NGOs, or civil society institutions has been established.</t>
-  </si>
-  <si>
-    <t>Roles of Women in the Value Chain
-1.	Involvement in Functions:
-o	Milking Animals: Women participate in milking.
-o	Maintaining Hygiene: Responsible for hygiene practices.
-o	Processing Products: Involved in boiling milk and other processing tasks.
-o	Selling Products: Sometimes sell dairy products in the market.
-2.	Functions Where Women Do Not Participate:
-o	Feeding Animals: Women do not engage in feeding livestock.
-o	Transporting Animal Waste: Not involved in this task.
-o	Treating Animals: Women do not participate in animal treatment.
-o	Buying and Selling Animals: Women typically do not engage in livestock trading in the market.</t>
-  </si>
-  <si>
-    <t>1.	Inputs:
-o	Animal Feed: Food materials such as straw, bran, chaff, breadcrumbs, and dried food for animal health.
-o	Health Supplies: Vaccines and medicinal herbs purchased from the market.
-2.	Production Steps:
-o	Milking: Collecting milk using buckets, barrels, or drums.
-o	Transportation: Using rented rickshaws or motorcycles for milk transport.
-3.	Outputs/Products:
-o	Dairy Products: Fresh milk and processed dairy items.
-4.	Value Addition Activities:
-o	Processing: Steps taken to boil milk and prepare other dairy products.
-o	Hygiene Maintenance: Ensuring cleanliness to maintain product quality.</t>
-  </si>
-  <si>
-    <t>Labor Force Involved in Operations
-1.	Actions/Processes Completed:
-o	Milking: Hand milking of animals.
-o	Processing: Preparing dairy products.
-o	Cleaning: Maintaining hygiene in the barn.
-o	Vaccinating Animals: Administering vaccines.
-o	Feeding Animals: Providing feed and water.
-o	Breeding Management: Overseeing animal breeding.
-o	Selling Products: Timing sales effectively.
-2.	Specific Skills:
-o	Hand Milking: Proficient in milking techniques.
-o	Processing Skills: Knowledge of dairy product preparation.
-o	Animal Nutrition: Understanding of proper feeding practices.
-3.	Involvement of Women:
-o	Tasks: Women participate in milking, cleaning, handling milking equipment, and selling products rarely.</t>
-  </si>
-  <si>
-    <t>Machinery Used in Operations
-1.	Current Machinery:
-o	Storage Containers: 
-	Types: 20-liter barrels, 40-liter, and 50-liter containers.
-	Actions: Used for storing milk.
-o	Processing Equipment: 
-	Types: Large ceramic bowls or pots.
-	Actions: Used for making fresh yogurt.
-o	Transportation: 
-	Type: local cars and zaranj.
-	Actions: Used for transporting dairy products.
-2.	Limitations:
-o	Modern Machinery: Not available due to high costs; the economy is weak.
-o	Financial Constraints: Basic production relies on manual labor.
-3.	Potential Needs:
-o	Desired Machinery: Milking machines, processing machines, storage tanks, freezers, and containers.
-o	Estimated Cost: At least 150,000 Afghanis for modern equipment.</t>
-  </si>
-  <si>
-    <t>Challenges in Selling Products/Services
-1.	Demand Changes:
-o	2024 vs. 2023: Demand for products has decreased due to widespread poverty and a low economic situation among the people. Continuous droughts have exacerbated economic challenges.
-2.	Identifying/Accessing Direct Buyers:
-o	Challenges: Lack of proper identification methods (signs or labels) hinders organized selling and access to buyers. Fixed collection points for milk are needed.
-3.	Meeting Buyer Requirements:
-o	Challenges: High demand for dairy products in summer, especially in sweet shops, but the inability to care for animals properly due to the high cost of animal feed limits production capacity.
-4.	Competition:
-o	Main Competitors: Foreign imports present significant competition.
-o	Level of Competition: Increased competition, especially during the fruit season when dairy products do not sell well, impacting overall sales.</t>
-  </si>
-  <si>
-    <t>Challenges in Accessing Necessary Inputs
-1.	Availability of Inputs:
-o	Food Items: Inputs are available but are expensive in the current market.
-o	Feed Quality: Available feed is of poor quality, failing to meet nutritional standards.
-2.	Affordability:
-o	High Costs: The expensive nature of inputs limits access, impacting overall operations and profitability.
-3.	Quality of Inputs:
-o	Nutritional Deficiencies: Current feed lacks essential protein, minerals, and other vital factors needed for animal health.
-o	Specific Requirements: Inputs do not meet the complete nutritional needs for optimal animal growth and production, leading to reduced productivity.
-Impact
-•	The inability to access affordable, high-quality inputs directly affects animal health and productivity, ultimately impacting the overall output of dairy products.</t>
-  </si>
-  <si>
-    <t>Challenges in Conducting Operational Processes
-1.	Equipment/Technology/Machinery Access:
-o	Hygiene Issues: Hand milking is not hygienic, leading to contamination with microbes during the milking process.
-o	Spillage Risks: Animals may kick over buckets or urinate, resulting in milk spoilage and loss of product.
-2.	Labor Skills:
-o	Lack of Training: There is a need for proper training and awareness regarding the use of milking machines and hygienic practices.
-o	Need for Facilities: A suitable milking area in the barn is essential to prevent contamination and improve efficiency.
-3.	Storage Needs:
-o	Temperature Control: Freezers are required to store milk and dairy products properly, especially in hot weather, to prevent spoilage.
-Impact on Business
-•	The challenges of unhygienic milking practices and lack of proper equipment lead to reduced product quality and increased spoilage, directly affecting sales and profitability. Additionally, the absence of training hinders the workforce's ability to operate machinery effectively, further limiting productivity and market competitiveness.</t>
-  </si>
-  <si>
-    <t>•	To address daily challenges effectively, we need good products, facilities, and machinery. Improving work methods, preventing unnecessary expenses, and raising awareness of new skills are essential for customer satisfaction.
-•	Enhancing the breed of local animals can increase production to meet market demand for dairy products year-round. Exporting our products to new markets would significantly boost our business.
-•	By improving animal breeds, understanding new markets, enhancing quality to meet standards, implementing marketing strategies, selecting appropriate sales methods, setting reasonable prices, and providing better services to international customers, we can achieve success. Additionally, utilizing suitable financial methods will contribute to sustainable growth.</t>
-  </si>
-  <si>
-    <t>Implementation Needs for Opportunities and Improvements
-1.	Financial Support:
-o	Purpose: We need financial support for purchasing machinery, improving livestock breeds, and expanding market infrastructure.
-o	Sources: Support should come from the government and relevant institutions.
-2.	Certifications:
-o	Standards: To ensure quality, we must meet specific certifications for dairy products, which may include health and safety standards for both production and export.
-3.	Technical Training:
-o	Training Needs: Essential training areas include: 
-	Animal care
-	Proper milk hygiene and delivery
-	Animal husbandry
-	Improved animal nutrition
-	Production management
-	Marketing methods
-	Use of modern machinery
-4.	Role of Government, NGOs, and Private Sector:
-o	Government: Facilitate financial support, establish training programs, and create infrastructure like milk collection centers.
-o	NGOs: Promote awareness and provide resources for quality dairy production and vaccination programs.</t>
-  </si>
-  <si>
-    <t>Missing Support Services and Challenges
-1.	Financial Services:
-o	Challenge: We lack access to financial services to support operations and investments.
-o	Impact: This limits our ability to purchase necessary equipment and improve livestock, hindering growth.
-2.	Transportation Services:
-o	Challenge: There are no reliable transportation services for distributing our dairy products.
-o	Impact: This affects our ability to reach markets efficiently, leading to potential losses and reduced sales.
-3.	Energy Access:
-o	Challenge: We do not have access to electricity or renewable energy sources like solar power.
-o	Impact: Lack of energy restricts the use of modern machinery and affects storage capabilities, risking product quality.
-4.	Marketing Development Services:
-o	Challenge: There is a deficiency in support for developing effective marketing strategies.
-o	Impact: Without proper marketing, we struggle to promote our products and reach potential customers.
-5.	Cooperation from Civil Institutions:
-o	Challenge: There is little cooperation from civil organizations and NGOs.
-o	Impact: This limits access to resources, training, and support programs that could enhance our operations.
-6.	High Costs:
-o	Challenge: High food prices increase operational costs.
-o	Impact: This reduces profit margins and makes it difficult to sustain operations.</t>
-  </si>
-  <si>
-    <t>Impact of the Business Environment on Operations
-1.	Regulations and Taxes:
-o	Current Status: There are no specific regulations or taxes imposed on our operations by the government.
-o	Impact: The absence of regulations allows for more flexibility in operations, but it also means a lack of support or guidelines that could enhance industry standards.
-2.	Climate Change:
-o	Impact: Climate change and drought conditions lead to decreased food supplies, affecting the availability of fodder and straw.
-o	Consequences: High prices for food products and scarcity in the market result in inadequate nutrition for our animals, which can decrease their productivity and overall health.</t>
-  </si>
-  <si>
-    <t>Changes Needed in Support Services and Business Environment
-1.	Animal Care and Nutrition:
-o	Change Needed: Implementation of advanced animal nutrition programs and improvements in animal genetics.
-o	Impact: This would ensure healthier livestock and increase milk production.
-2.	Advanced Machinery:
-o	Change Needed: Access to modern machinery for dairy production, storage, and transportation.
-o	Impact: Enhanced efficiency in production processes and better preservation of product quality during transport.
-3.	Livestock Management Training:
-o	Change Needed: Comprehensive training programs in livestock management, processing, and packaging.
-o	Impact: Improved skills among farmers, leading to better product quality and operational efficiency.
-4.	Promotion of Dairy Consumption:
-o	Change Needed: Initiatives to promote the daily consumption of dairy products.
-o	Impact: Increased demand for dairy products, benefiting producers.
-5.	Sales Locations:
-o	Change Needed: Development of suitable sales locations for dairy products.
-o	Impact: Enhanced accessibility for consumers, leading to increased sales.
-6.	Government and Institutional Support:
-o	Change Needed: Stronger support from government and institutions in the form of funding, training, and infrastructure development.
-o	Impact: Essential for growth, enabling producers to improve product quality and meet market demands.</t>
-  </si>
-  <si>
-    <t>1.	Grazing Space:
-o	Issue: There is a lack of suitable grazing areas for livestock.
-o	Impact: Limited grazing space can lead to overgrazing and poor animal health due to inadequate nutrition.
-2.	Water Access:
-o	Issue: Access to clean and sufficient water for livestock is a challenge.
-o	Impact: Insufficient water supply directly affects animal health and productivity.
-3.	Animal Care Challenges:
-o	Issue: There are ongoing difficulties in providing comprehensive care for animals.
-o	Impact: Poor animal care can lead to health issues, reducing milk production and quality.
-4.	Handling and Transporting Animal Waste:
-o	Issue: Efficient management of animal waste is problematic.
-o	Impact: Challenges in waste handling can lead to environmental concerns and increased operational costs.</t>
   </si>
   <si>
     <t>Abdul Sami Yaqobi</t>
@@ -839,9 +546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -858,7 +563,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -869,7 +574,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -877,10 +582,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>68</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -888,10 +593,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -899,10 +604,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -910,10 +615,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -921,10 +626,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -932,10 +637,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -943,10 +648,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>72</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -954,10 +659,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="395" x14ac:dyDescent="0.2">
@@ -965,10 +670,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
@@ -976,165 +681,81 @@
         <v>12</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="365" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="208" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="240" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="335" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="288" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="380" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="256" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="365" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="320" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="395" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="240" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="288" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>67</v>
-      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1371,15 +992,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="fcf89adc-eefc-4033-818a-934b0690d419" xsi:nil="true"/>
@@ -1390,14 +1002,49 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C433EF18-CC8B-454E-9619-870C5EF7F6D9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C433EF18-CC8B-454E-9619-870C5EF7F6D9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6b197b6a-cffc-4ca7-9de0-77d82e42a5a9"/>
+    <ds:schemaRef ds:uri="fcf89adc-eefc-4033-818a-934b0690d419"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27E48472-2410-49A3-A9C1-5B22521789D5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D8E771A-9030-46EA-BDE1-796E49D140C3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fcf89adc-eefc-4033-818a-934b0690d419"/>
+    <ds:schemaRef ds:uri="6b197b6a-cffc-4ca7-9de0-77d82e42a5a9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D8E771A-9030-46EA-BDE1-796E49D140C3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27E48472-2410-49A3-A9C1-5B22521789D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>